<commit_message>
0.8.2 - Start of Office day. Made some changes to backend due to crashing
</commit_message>
<xml_diff>
--- a/keel_vessel_import_template.xlsx
+++ b/keel_vessel_import_template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F20D333-1E6E-4623-9B29-11D071660BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D51AD58-F8FA-45AC-B8EC-6C811F497843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vessels" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="82">
   <si>
     <t>imo_number</t>
   </si>
@@ -638,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E27"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,255 +671,255 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
+      <c r="A2">
+        <v>9101112</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9101112</v>
+        <v>9102223</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>9102223</v>
+        <v>9103334</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>9103334</v>
+        <v>9104445</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>9104445</v>
+        <v>9105556</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>9105556</v>
+        <v>9106667</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9106667</v>
+        <v>9107778</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9107778</v>
+        <v>9108889</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9108889</v>
+        <v>9109990</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9109990</v>
+        <v>9110001</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>9110001</v>
+        <v>9111112</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9111112</v>
+        <v>9112223</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>9112223</v>
+        <v>9113334</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>9113334</v>
+        <v>9114445</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>9114445</v>
+        <v>9115556</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>36</v>
@@ -927,188 +927,171 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>9115556</v>
+        <v>9116667</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>9116667</v>
+        <v>9117778</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>9117778</v>
+        <v>9118889</v>
       </c>
       <c r="B19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>9118889</v>
+        <v>9119990</v>
       </c>
       <c r="B20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>9119990</v>
+        <v>9120001</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>9120001</v>
+        <v>9121112</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>9121112</v>
+        <v>9122223</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>9122223</v>
+        <v>9123334</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9123334</v>
+        <v>9124445</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>9124445</v>
+        <v>9125556</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="E26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9125556</v>
-      </c>
-      <c r="B27" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E27" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1122,13 +1105,13 @@
           <x14:formula1>
             <xm:f>_meta!$A$1:$A$11</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C1000</xm:sqref>
+          <xm:sqref>C2:C999</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Class Society" error="Please select a valid Class Society from the dropdown list." xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>_meta!$B$1:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1000</xm:sqref>
+          <xm:sqref>E2:E999</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>